<commit_message>
updates to app for retinopathy
</commit_message>
<xml_diff>
--- a/Documentation/Demo_Entries_Details.xlsx
+++ b/Documentation/Demo_Entries_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edwar\Desktop\Projects\Utterly_Uncreative_2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E3FA46-A71D-4B2E-AF3A-2BAC95FFB07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E5D8FA-4DA4-4E7B-903E-EEDDDE2992BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{0B4F660A-6924-4F2C-9A63-5C67D3C4F165}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="53">
   <si>
     <t>id_code</t>
   </si>
@@ -151,6 +151,39 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Screen Location</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>2,5</t>
   </si>
 </sst>
 </file>
@@ -303,15 +336,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -340,6 +370,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -655,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D359B68E-4781-4B69-AC1F-DDF084D073D1}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,56 +708,60 @@
     <col min="7" max="7" width="5.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.26953125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="10" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="12"/>
-    </row>
-    <row r="2" spans="1:9" ht="28" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:10" ht="56" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
         <v>190</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2">
@@ -733,25 +773,28 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <f t="shared" ref="H3:H27" si="0">G3-C3</f>
         <v>0</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="1">
+      <c r="J3" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
         <v>279</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2">
@@ -763,21 +806,24 @@
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I4" s="2">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>296</v>
       </c>
@@ -793,25 +839,26 @@
       <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="2">
         <v>3</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I5" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="1">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
         <v>312</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2">
@@ -823,21 +870,24 @@
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I6" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>465</v>
       </c>
@@ -853,21 +903,22 @@
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="2">
         <v>4</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I7" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>492</v>
       </c>
@@ -883,21 +934,22 @@
       <c r="E8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G8" s="2">
         <v>2</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I8" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>619</v>
       </c>
@@ -913,21 +965,22 @@
       <c r="E9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G9" s="2">
         <v>2</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I9" s="2">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>671</v>
       </c>
@@ -943,25 +996,26 @@
       <c r="E10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="I10" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="1">
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A11" s="12">
         <v>700</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="2">
@@ -973,21 +1027,24 @@
       <c r="E11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="2">
         <v>3</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I11" s="2">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>1046</v>
       </c>
@@ -1003,25 +1060,26 @@
       <c r="E12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="2">
         <v>0</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I12" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" s="1">
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A13" s="12">
         <v>1097</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="2">
@@ -1033,25 +1091,28 @@
       <c r="E13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F13" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="2">
         <v>4</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I13" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" s="1">
+      <c r="J13" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="12">
         <v>1225</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C14" s="2">
@@ -1063,25 +1124,28 @@
       <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G14" s="2">
         <v>2</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14" s="2">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="J14" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A15" s="12">
         <v>1289</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="2">
@@ -1093,21 +1157,24 @@
       <c r="E15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G15" s="2">
         <v>1</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J15" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1619</v>
       </c>
@@ -1123,21 +1190,22 @@
       <c r="E16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
       <c r="G16" s="2">
         <v>2</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I16" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2188</v>
       </c>
@@ -1153,21 +1221,22 @@
       <c r="E17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="2">
         <v>1</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I17" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>2255</v>
       </c>
@@ -1183,21 +1252,22 @@
       <c r="E18" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G18" s="2">
         <v>2</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="4">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I18" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>2521</v>
       </c>
@@ -1213,21 +1283,22 @@
       <c r="E19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G19" s="2">
         <v>3</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19" s="2">
         <v>23</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>2708</v>
       </c>
@@ -1243,25 +1314,26 @@
       <c r="E20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="F20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G20" s="2">
         <v>1</v>
       </c>
-      <c r="H20" s="4">
+      <c r="H20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I20" s="2">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A21" s="1">
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" s="12">
         <v>2713</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C21" s="2">
@@ -1273,21 +1345,24 @@
       <c r="E21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G21" s="2">
         <v>3</v>
       </c>
-      <c r="H21" s="4">
+      <c r="H21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I21" s="2">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J21" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>2818</v>
       </c>
@@ -1303,25 +1378,26 @@
       <c r="E22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="2">
         <v>0</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I22" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A23" s="1">
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A23" s="12">
         <v>3063</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C23" s="2">
@@ -1333,21 +1409,24 @@
       <c r="E23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G23" s="2">
         <v>4</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I23" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J23" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>3228</v>
       </c>
@@ -1363,21 +1442,22 @@
       <c r="E24" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G24" s="2">
         <v>2</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="4">
         <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="I24" s="2">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>3291</v>
       </c>
@@ -1393,25 +1473,26 @@
       <c r="E25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="2">
         <v>0</v>
       </c>
-      <c r="H25" s="4">
+      <c r="H25" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I25" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="1">
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="12">
         <v>3296</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="2">
@@ -1423,21 +1504,24 @@
       <c r="E26" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G26" s="2">
         <v>0</v>
       </c>
-      <c r="H26" s="4">
+      <c r="H26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I26" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J26" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>3453</v>
       </c>
@@ -1453,19 +1537,20 @@
       <c r="E27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="4" t="s">
+      <c r="F27" s="3" t="s">
         <v>14</v>
       </c>
       <c r="G27" s="2">
         <v>4</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H27" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I27" s="2">
         <v>20</v>
       </c>
+      <c r="J27" s="2"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:H27">

</xml_diff>